<commit_message>
Issue #17: Updates related work.
</commit_message>
<xml_diff>
--- a/resources/snowballing.xlsx
+++ b/resources/snowballing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessa/workspace/db-mining/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440D421B-3530-D34E-904F-18A189E141F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C41CE2B-3239-404B-9E69-F081CCEC7990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1955" uniqueCount="1401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="1402">
   <si>
     <t>authors</t>
   </si>
@@ -5531,6 +5531,9 @@
   </si>
   <si>
     <t>paper_relevant</t>
+  </si>
+  <si>
+    <t>Paper deals with databases to support software development -- focus is not on user application, but on SE tools</t>
   </si>
 </sst>
 </file>
@@ -5566,7 +5569,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5581,6 +5584,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6F0CF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5613,7 +5622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5628,12 +5637,104 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6033,10 +6134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01F3603-C7EC-6148-A061-EC7A3953FAAF}">
-  <dimension ref="A1:M261"/>
+  <dimension ref="A1:N261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I131" sqref="I131"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8236,7 +8337,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>443</v>
       </c>
@@ -8262,7 +8363,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>300</v>
       </c>
@@ -8288,7 +8389,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>716</v>
       </c>
@@ -8314,7 +8415,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>617</v>
       </c>
@@ -8340,7 +8441,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>510</v>
       </c>
@@ -8366,7 +8467,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>344</v>
       </c>
@@ -8392,7 +8493,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>860</v>
       </c>
@@ -8421,7 +8522,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>943</v>
       </c>
@@ -8450,7 +8551,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>905</v>
       </c>
@@ -8479,7 +8580,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>304</v>
       </c>
@@ -8505,7 +8606,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1219</v>
       </c>
@@ -8534,7 +8635,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>890</v>
       </c>
@@ -8563,7 +8664,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>642</v>
       </c>
@@ -8589,17 +8690,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+    <row r="94" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="10" t="s">
         <v>850</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="11" t="s">
         <v>1092</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="10" t="s">
         <v>851</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="10" t="s">
         <v>852</v>
       </c>
       <c r="E94" t="s">
@@ -8617,8 +8718,20 @@
       <c r="I94" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="J94" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="N94" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>794</v>
       </c>
@@ -8644,7 +8757,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>875</v>
       </c>
@@ -9600,16 +9713,16 @@
       </c>
     </row>
     <row r="131" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="A131" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="6" t="s">
         <v>1089</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="3" t="s">
         <v>837</v>
       </c>
       <c r="E131" t="s">
@@ -12573,16 +12686,16 @@
       </c>
     </row>
     <row r="239" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A239" t="s">
+      <c r="A239" s="3" t="s">
         <v>1119</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B239" s="3" t="s">
         <v>1120</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C239" s="3" t="s">
         <v>1121</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D239" s="3" t="s">
         <v>1122</v>
       </c>
       <c r="E239" t="s">
@@ -13226,25 +13339,58 @@
     <sortCondition ref="D3:D256"/>
   </sortState>
   <conditionalFormatting sqref="I2">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Maybe">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Maybe">
       <formula>NOT(ISERROR(SEARCH("Maybe",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I261">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Maybe">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Maybe">
       <formula>NOT(ISERROR(SEARCH("Maybe",I3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",I3)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",I3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J94">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Maybe">
+      <formula>NOT(ISERROR(SEARCH("Maybe",J94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",J94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",J94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K94">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Maybe">
+      <formula>NOT(ISERROR(SEARCH("Maybe",K94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",K94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",K94)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M94">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Maybe">
+      <formula>NOT(ISERROR(SEARCH("Maybe",M94)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",M94)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",I3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("No",M94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>